<commit_message>
Added more validation steps of data entered by users.
</commit_message>
<xml_diff>
--- a/Python-RandomForest/Python_Random_Forest/data/AssayType_DesiredResults_UsedColumns.xlsx
+++ b/Python-RandomForest/Python_Random_Forest/data/AssayType_DesiredResults_UsedColumns.xlsx
@@ -3,20 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PHARTEN\git\nanoQSAR\Python-RandomForest\Python_Random_Forest\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DED26B-3D16-4F8B-BD4A-6E491C0DBE70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{FF1C032D-B2FE-4D9D-8732-F32A1DFAC2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4608" yWindow="0" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2184" yWindow="0" windowWidth="18612" windowHeight="12012" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AssayType_DesiredResults_UsedCo" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="N1:Q15"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9695" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9715" uniqueCount="130">
   <si>
     <t>CoreComposition</t>
   </si>
@@ -413,6 +409,15 @@
   </si>
   <si>
     <t>Cerium(IV) oxide</t>
+  </si>
+  <si>
+    <t>micrometers</t>
+  </si>
+  <si>
+    <t>square centimeters/gram</t>
+  </si>
+  <si>
+    <t>fraction</t>
   </si>
 </sst>
 </file>
@@ -1257,9 +1262,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CD440"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1271,7 +1276,7 @@
     <col min="5" max="5" width="17.77734375" style="2" customWidth="1"/>
     <col min="6" max="6" width="16.88671875" style="2" customWidth="1"/>
     <col min="7" max="7" width="16.109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="17.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" style="1" customWidth="1"/>
     <col min="9" max="10" width="15.33203125" customWidth="1"/>
     <col min="11" max="11" width="12.44140625" customWidth="1"/>
     <col min="13" max="13" width="10.21875" customWidth="1"/>
@@ -1599,16 +1604,61 @@
       <c r="B2" s="1" t="s">
         <v>99</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="M2" t="s">
+        <v>86</v>
+      </c>
+      <c r="O2" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="3" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
+        <v>85</v>
+      </c>
+      <c r="R3" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="4" spans="1:82" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>123</v>
       </c>
+      <c r="C4" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G4" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="K4" t="s">
+        <v>119</v>
+      </c>
+      <c r="M4" t="s">
+        <v>129</v>
+      </c>
+      <c r="O4" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="5" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -28040,10 +28090,24 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="C2:C5 E2:F5 N2:N5 P2:Q5" xr:uid="{2E127230-C05D-43EC-BD0E-0ED188DC4ADB}">
+      <formula1>0</formula1>
+      <formula2>1000</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="G2:G5 I2:J5" xr:uid="{2951C693-7123-4FEE-89B0-6C5FF1EBAC3C}">
+      <formula1>0</formula1>
+      <formula2>10000</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L5" xr:uid="{6338EA1D-E03D-4F5C-89A1-117C4601F40F}">
+      <formula1>0</formula1>
+      <formula2>100</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{9EF790BF-0A90-4D8B-A831-209FD6971A87}">
           <x14:formula1>
             <xm:f>Sheet1!$A$440:$A$448</xm:f>
@@ -28056,6 +28120,36 @@
           </x14:formula1>
           <xm:sqref>B2:B5</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{9866106B-EADE-4603-BE0F-5C96FB1B7AC1}">
+          <x14:formula1>
+            <xm:f>Sheet1!$D$440:$D$442</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D5 O2:O5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{965B1D26-7389-4956-8C23-7D54CFD312F4}">
+          <x14:formula1>
+            <xm:f>Sheet1!$H$440:$H$442</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{18B3E6BA-200C-444F-AA20-AAB952A02FB8}">
+          <x14:formula1>
+            <xm:f>Sheet1!$K$440:$K$442</xm:f>
+          </x14:formula1>
+          <xm:sqref>K2:K5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{E05E1AE9-9A25-49AE-873B-BEB4B22254AE}">
+          <x14:formula1>
+            <xm:f>Sheet1!$M$440:$M$442</xm:f>
+          </x14:formula1>
+          <xm:sqref>M2:M5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{705E517F-1E39-4D65-ABEE-040917C1BCDE}">
+          <x14:formula1>
+            <xm:f>Sheet1!$R$440:$R$441</xm:f>
+          </x14:formula1>
+          <xm:sqref>R2:R5</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -28066,8 +28160,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0CEAD00-67BB-4B6C-8616-8F41E3EDC171}">
   <dimension ref="A1:CD448"/>
   <sheetViews>
-    <sheetView topLeftCell="A428" workbookViewId="0">
-      <selection activeCell="B441" sqref="B441"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A427" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="N1" sqref="N1"/>
+      <selection pane="bottomLeft" activeCell="R441" sqref="R441"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28079,7 +28175,7 @@
     <col min="5" max="5" width="17.77734375" style="2" customWidth="1"/>
     <col min="6" max="6" width="16.88671875" style="2" customWidth="1"/>
     <col min="7" max="7" width="16.109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="17.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21" style="1" customWidth="1"/>
     <col min="9" max="10" width="15.33203125" customWidth="1"/>
     <col min="11" max="11" width="12.44140625" customWidth="1"/>
     <col min="13" max="13" width="10.21875" customWidth="1"/>
@@ -54828,6 +54924,21 @@
       <c r="B441" s="1" t="s">
         <v>99</v>
       </c>
+      <c r="D441" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H441" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="K441" t="s">
+        <v>85</v>
+      </c>
+      <c r="M441" t="s">
+        <v>86</v>
+      </c>
+      <c r="R441" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="442" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A442" s="1" t="s">
@@ -54835,6 +54946,18 @@
       </c>
       <c r="B442" s="1" t="s">
         <v>102</v>
+      </c>
+      <c r="D442" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H442" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="K442" t="s">
+        <v>119</v>
+      </c>
+      <c r="M442" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="443" spans="1:77" x14ac:dyDescent="0.3">

</xml_diff>